<commit_message>
i think its working better
</commit_message>
<xml_diff>
--- a/projects/DC_analysis/PTool_leds.xlsx
+++ b/projects/DC_analysis/PTool_leds.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2137,9 +2137,6 @@
     <t>[0,1]</t>
   </si>
   <si>
-    <t>diag</t>
-  </si>
-  <si>
     <t>diagonal</t>
   </si>
   <si>
@@ -2204,6 +2201,9 @@
   </si>
   <si>
     <t>Ptool LEDs</t>
+  </si>
+  <si>
+    <t>single_run</t>
   </si>
 </sst>
 </file>
@@ -6433,8 +6433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6492,7 +6492,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6503,7 +6503,7 @@
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
@@ -6574,7 +6574,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6585,7 +6585,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="31" t="s">
@@ -6677,7 +6677,7 @@
         <v>451</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>698</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6706,10 +6706,10 @@
         <v>691</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D25" s="33"/>
     </row>
@@ -6786,7 +6786,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6869,9 +6869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7050,7 +7050,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>681</v>
@@ -7065,10 +7065,10 @@
         <v>694</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="P5" s="31" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="R5" s="31" t="s">
         <v>693</v>
@@ -7076,13 +7076,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B6" s="31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>685</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>682</v>
@@ -7106,7 +7106,7 @@
         <v>684</v>
       </c>
       <c r="P6" s="31" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="R6" s="31" t="s">
         <v>693</v>
@@ -7114,7 +7114,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>688</v>
@@ -7144,7 +7144,7 @@
         <v>689</v>
       </c>
       <c r="P7" s="50" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="R7" s="31" t="s">
         <v>693</v>
@@ -7155,13 +7155,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="36" t="s">
+        <v>712</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>713</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>714</v>
-      </c>
       <c r="D8" s="36" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>68</v>
@@ -7172,7 +7172,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>696</v>
@@ -7181,7 +7181,7 @@
         <v>65</v>
       </c>
       <c r="I9" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="31"/>
       <c r="K9" s="31">
@@ -8214,12 +8214,12 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>468</v>
@@ -8620,14 +8620,14 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="39" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C21" s="39"/>
       <c r="D21" s="39" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="39" t="s">
@@ -8649,14 +8649,14 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="39" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C22" s="39"/>
       <c r="D22" s="39" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="39" t="s">

</xml_diff>